<commit_message>
Running script using POM SEP branch 01
</commit_message>
<xml_diff>
--- a/zoom12/resources/utils/zoom12User.xlsx
+++ b/zoom12/resources/utils/zoom12User.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9720" windowHeight="3870"/>
+    <workbookView windowWidth="13785" windowHeight="3570"/>
   </bookViews>
   <sheets>
     <sheet name="zoom12Users" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Passwords</t>
+  </si>
   <si>
     <t>zoomtest18@mailinator.com</t>
   </si>
@@ -26,19 +32,10 @@
     <t>zoomtest19@mailinator.com</t>
   </si>
   <si>
-    <t>Password$124</t>
-  </si>
-  <si>
     <t>zoomtest20@mailinator.com</t>
   </si>
   <si>
-    <t>Password$125</t>
-  </si>
-  <si>
     <t>zoomtest21@mailinator.com</t>
-  </si>
-  <si>
-    <t>Password$126</t>
   </si>
 </sst>
 </file>
@@ -47,9 +44,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -61,6 +58,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -69,7 +73,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -83,9 +94,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,61 +109,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,6 +140,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -182,6 +163,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -189,16 +186,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,13 +216,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,7 +294,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,151 +354,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,13 +419,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,6 +458,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -472,30 +482,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -504,153 +490,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -663,10 +660,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
-    <cellStyle name="Currency[0]" xfId="6" builtinId="7"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
     <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
     <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
     <cellStyle name="Note" xfId="9" builtinId="10"/>
@@ -711,6 +708,11 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -966,20 +968,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B4"/>
+      <selection activeCell="A7" sqref="$A7:$XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1002,15 +1006,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>